<commit_message>
Roster Pattern Setup ( Create, Update, Deactivate)
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Jivi_Test_Data.xlsx
+++ b/src/test/resources/TestData/Jivi_Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Test_Case_ Skill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E503D61F-D80C-4385-9F7E-146B2F78747F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75B3B9F-849C-4D39-8472-01CDB1B6AE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{FD64DE87-D4F6-4997-BAAC-D24454267BB6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="83">
   <si>
     <t>admin</t>
   </si>
@@ -290,25 +290,22 @@
     </r>
   </si>
   <si>
-    <t>roasterSetupTest</t>
-  </si>
-  <si>
-    <t>verifyCreateRoaster</t>
-  </si>
-  <si>
     <t>shiftBandTest</t>
   </si>
   <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>14 days pattern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 days pattern  Description </t>
-  </si>
-  <si>
-    <t>updateCreateRoaster</t>
+    <t>No of Blocks</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>verifyCreateRoster</t>
+  </si>
+  <si>
+    <t>updateCreateRoster</t>
+  </si>
+  <si>
+    <t>rosterSetupTest</t>
   </si>
 </sst>
 </file>
@@ -490,6 +487,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -517,7 +515,6 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal 1" xfId="1" xr:uid="{41565CED-8248-4079-BB1E-AB6BDFDF14B2}"/>
@@ -835,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{882E081F-02C7-46D7-AF78-5A47B331B7E3}">
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -967,7 +964,7 @@
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="17" t="s">
         <v>32</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -993,7 +990,7 @@
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="2" t="s">
         <v>29</v>
       </c>
@@ -1025,7 +1022,7 @@
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="18"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="2" t="s">
         <v>29</v>
       </c>
@@ -1083,7 +1080,7 @@
       <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="17" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1119,7 +1116,7 @@
       <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="18"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="2" t="s">
         <v>33</v>
       </c>
@@ -1193,11 +1190,11 @@
       <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="20" t="s">
         <v>32</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>46</v>
@@ -1245,9 +1242,9 @@
       <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="20"/>
+      <c r="B11" s="21"/>
       <c r="C11" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>47</v>
@@ -1295,9 +1292,9 @@
       <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="21"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>48</v>
@@ -1339,7 +1336,7 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>52</v>
@@ -1406,7 +1403,9 @@
       <c r="J14" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="K14" s="11"/>
+      <c r="K14" s="11" t="s">
+        <v>78</v>
+      </c>
       <c r="L14" s="11"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -1421,14 +1420,14 @@
       <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="23" t="s">
         <v>76</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>0</v>
@@ -1446,9 +1445,11 @@
       <c r="J15" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K15" s="1"/>
+      <c r="K15" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="L15" s="1"/>
-      <c r="M15" s="25"/>
+      <c r="M15" s="16"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -1461,12 +1462,12 @@
       <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="23"/>
+      <c r="B16" s="24"/>
       <c r="C16" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>0</v>
@@ -1475,20 +1476,16 @@
         <v>1</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="H16" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="K16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B17" s="24"/>
+      <c r="B17" s="25"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>

</xml_diff>

<commit_message>
SCR ( Create, Update, Deactive )
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Jivi_Test_Data.xlsx
+++ b/src/test/resources/TestData/Jivi_Test_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Test_Case_ Skill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75B3B9F-849C-4D39-8472-01CDB1B6AE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FAB8CA-00E9-4421-A076-1975B4CFE685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{FD64DE87-D4F6-4997-BAAC-D24454267BB6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="129">
   <si>
     <t>admin</t>
   </si>
@@ -306,6 +306,144 @@
   </si>
   <si>
     <t>rosterSetupTest</t>
+  </si>
+  <si>
+    <t>Holiday Name</t>
+  </si>
+  <si>
+    <t>Holiday Date</t>
+  </si>
+  <si>
+    <t>Holiday Note</t>
+  </si>
+  <si>
+    <t>publicHolidayTest</t>
+  </si>
+  <si>
+    <t>verifyCreatePublicHoliday</t>
+  </si>
+  <si>
+    <t>New Year</t>
+  </si>
+  <si>
+    <t>01/01/2024</t>
+  </si>
+  <si>
+    <t>New Year Leave</t>
+  </si>
+  <si>
+    <t>Christmas</t>
+  </si>
+  <si>
+    <t>25/12/2023</t>
+  </si>
+  <si>
+    <t>Christmas Leave</t>
+  </si>
+  <si>
+    <t>verifyUpdatePublicHoliday</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valid From </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valid To </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Period Length </t>
+  </si>
+  <si>
+    <t>Shift Length Min</t>
+  </si>
+  <si>
+    <t>Shift Length Max</t>
+  </si>
+  <si>
+    <t>Cont Working Days-Min</t>
+  </si>
+  <si>
+    <t>Cont Working Days-Max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Days Per Period_Min </t>
+  </si>
+  <si>
+    <t>Days Per Period -Max</t>
+  </si>
+  <si>
+    <t>Time per period _Max</t>
+  </si>
+  <si>
+    <t>Cont. Working Days - Min</t>
+  </si>
+  <si>
+    <t>Cont. Working Days - Max</t>
+  </si>
+  <si>
+    <t>Cont. Off Days - Min.</t>
+  </si>
+  <si>
+    <t>Cont. Off Days - Max.</t>
+  </si>
+  <si>
+    <t>Shift Band Per Period - Min</t>
+  </si>
+  <si>
+    <t>Shift Band Per Period - Max</t>
+  </si>
+  <si>
+    <t>Min. Rest Hours</t>
+  </si>
+  <si>
+    <t>JiviewsAutomation.SystemDefination_Test</t>
+  </si>
+  <si>
+    <t>Deafault SCR</t>
+  </si>
+  <si>
+    <t>1/08/2023</t>
+  </si>
+  <si>
+    <t>10:00</t>
+  </si>
+  <si>
+    <t>12:00</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Cont off Days-Min</t>
+  </si>
+  <si>
+    <t>Cont off Days-Max</t>
+  </si>
+  <si>
+    <t>Time per Period-Min</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>verifyCreateSCR</t>
+  </si>
+  <si>
+    <t>SCRTest</t>
+  </si>
+  <si>
+    <t>Spacial SCR</t>
+  </si>
+  <si>
+    <t>setUpdateSCR</t>
   </si>
 </sst>
 </file>
@@ -464,7 +602,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -488,6 +626,14 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -504,15 +650,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -830,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{882E081F-02C7-46D7-AF78-5A47B331B7E3}">
-  <dimension ref="A1:U17"/>
+  <dimension ref="A1:AC24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="C11" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -841,7 +978,7 @@
     <col min="1" max="1" width="8.7265625" style="5"/>
     <col min="2" max="2" width="44.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.36328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
@@ -850,16 +987,26 @@
     <col min="10" max="10" width="15.81640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.26953125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.08984375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="24.90625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5">
         <v>0</v>
       </c>
@@ -923,8 +1070,32 @@
       <c r="U1" s="4">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V1" s="4">
+        <v>21</v>
+      </c>
+      <c r="W1" s="4">
+        <v>22</v>
+      </c>
+      <c r="X1" s="4">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="4">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="4">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="4">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="4">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -960,11 +1131,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="21" t="s">
         <v>32</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -986,11 +1157,11 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="18"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="2" t="s">
         <v>29</v>
       </c>
@@ -1018,11 +1189,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="19"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="2" t="s">
         <v>29</v>
       </c>
@@ -1050,7 +1221,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1076,11 +1247,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="21" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1112,11 +1283,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="19"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="2" t="s">
         <v>33</v>
       </c>
@@ -1136,7 +1307,7 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1186,11 +1357,11 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1238,11 +1409,11 @@
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="21"/>
+      <c r="B11" s="25"/>
       <c r="C11" s="2" t="s">
         <v>77</v>
       </c>
@@ -1288,11 +1459,11 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="22"/>
+      <c r="B12" s="25"/>
       <c r="C12" s="2" t="s">
         <v>77</v>
       </c>
@@ -1330,11 +1501,11 @@
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="2" t="s">
         <v>77</v>
       </c>
@@ -1384,7 +1555,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1416,11 +1587,11 @@
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="19" t="s">
         <v>76</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1458,11 +1629,11 @@
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="24"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="2" t="s">
         <v>82</v>
       </c>
@@ -1484,25 +1655,315 @@
       </c>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B17" s="25"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="K18" s="3"/>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="20"/>
+      <c r="C19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="K19" s="17"/>
+      <c r="L19" s="18"/>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="L20" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="M20" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="N20" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="O20" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="P20" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q20" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="R20" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="S20" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="T20" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="U20" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="V20" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="W20" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="X20" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y20" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z20" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA20" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB20" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC20" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="K21" s="1"/>
+      <c r="L21" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="P21" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q21" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="R21" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="S21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="U21" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="V21" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="W21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="X21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA21" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB21" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC21" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="20"/>
+      <c r="C22" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="1"/>
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="1"/>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B18:B19"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B10:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
SkillSetUpTest, RoleSetUpTest, RoleGroupTest, ShiftBandTest, SCRTest, PublicHolidayTest
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Jivi_Test_Data.xlsx
+++ b/src/test/resources/TestData/Jivi_Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Test_Case_ Skill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FD8B4C-E61C-4D74-BC27-662E9569134B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59FC7BC-26E3-4B3F-B89F-7AF392ECC480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{FD64DE87-D4F6-4997-BAAC-D24454267BB6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="138">
   <si>
     <t>admin</t>
   </si>
@@ -465,6 +465,12 @@
   </si>
   <si>
     <t>QCO Operator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QCO </t>
+  </si>
+  <si>
+    <t>QCO</t>
   </si>
 </sst>
 </file>
@@ -649,6 +655,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -671,9 +680,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -993,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{882E081F-02C7-46D7-AF78-5A47B331B7E3}">
   <dimension ref="A1:AC30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1159,7 +1165,7 @@
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="22" t="s">
         <v>32</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1185,7 +1191,7 @@
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="22"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="2" t="s">
         <v>29</v>
       </c>
@@ -1217,7 +1223,7 @@
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="23"/>
+      <c r="B5" s="24"/>
       <c r="C5" s="2" t="s">
         <v>29</v>
       </c>
@@ -1275,7 +1281,7 @@
       <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="22" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1311,7 +1317,7 @@
       <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="23"/>
+      <c r="B8" s="24"/>
       <c r="C8" s="2" t="s">
         <v>33</v>
       </c>
@@ -1325,10 +1331,18 @@
         <v>1</v>
       </c>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.35">
@@ -1385,7 +1399,7 @@
       <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="25" t="s">
         <v>32</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1437,7 +1451,7 @@
       <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="25"/>
+      <c r="B11" s="26"/>
       <c r="C11" s="2" t="s">
         <v>77</v>
       </c>
@@ -1487,7 +1501,7 @@
       <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="25"/>
+      <c r="B12" s="26"/>
       <c r="C12" s="2" t="s">
         <v>77</v>
       </c>
@@ -1529,7 +1543,7 @@
       <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="26"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="2" t="s">
         <v>77</v>
       </c>
@@ -1615,7 +1629,7 @@
       <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="20" t="s">
         <v>76</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1657,7 +1671,7 @@
       <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="20"/>
+      <c r="B16" s="21"/>
       <c r="C16" s="2" t="s">
         <v>82</v>
       </c>
@@ -1705,7 +1719,7 @@
       <c r="A18" s="5">
         <v>17</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="20" t="s">
         <v>76</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -1737,7 +1751,7 @@
       <c r="A19" s="5">
         <v>18</v>
       </c>
-      <c r="B19" s="20"/>
+      <c r="B19" s="21"/>
       <c r="C19" s="2" t="s">
         <v>86</v>
       </c>
@@ -1844,7 +1858,7 @@
       <c r="A21" s="5">
         <v>20</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="20" t="s">
         <v>114</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -1929,7 +1943,7 @@
       <c r="A22" s="5">
         <v>21</v>
       </c>
-      <c r="B22" s="20"/>
+      <c r="B22" s="21"/>
       <c r="C22" s="1" t="s">
         <v>126</v>
       </c>
@@ -1990,7 +2004,7 @@
       <c r="A24" s="5">
         <v>23</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="19" t="s">
         <v>114</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -2016,7 +2030,7 @@
       <c r="A25" s="5">
         <v>24</v>
       </c>
-      <c r="B25" s="27"/>
+      <c r="B25" s="19"/>
       <c r="C25" s="1" t="s">
         <v>131</v>
       </c>
@@ -2040,7 +2054,7 @@
       <c r="A26" s="5">
         <v>25</v>
       </c>
-      <c r="B26" s="27"/>
+      <c r="B26" s="19"/>
       <c r="C26" s="1" t="s">
         <v>131</v>
       </c>

</xml_diff>